<commit_message>
Fixed a bug in the HMM model for normalizing zero likelihood. Report draft 0.
</commit_message>
<xml_diff>
--- a/a3/perf.xlsx
+++ b/a3/perf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="4260" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="perf" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
   <si>
     <t>null likelihood</t>
   </si>
@@ -113,8 +113,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -153,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -170,6 +188,15 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -186,6 +213,15 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1019,8 +1055,14 @@
       <c r="A25" t="s">
         <v>12</v>
       </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
       <c r="C25">
         <v>10</v>
+      </c>
+      <c r="D25">
+        <v>30</v>
       </c>
       <c r="E25">
         <v>0.24985754985754899</v>
@@ -1042,8 +1084,14 @@
       <c r="A26" t="s">
         <v>12</v>
       </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
       <c r="C26">
         <v>100</v>
+      </c>
+      <c r="D26">
+        <v>30</v>
       </c>
       <c r="E26">
         <v>0.207549857549857</v>
@@ -1065,8 +1113,14 @@
       <c r="A27" t="s">
         <v>12</v>
       </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
       <c r="C27">
         <v>1000</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
       </c>
       <c r="E27">
         <v>0.221082621082621</v>
@@ -1088,8 +1142,14 @@
       <c r="A28" t="s">
         <v>12</v>
       </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
       <c r="C28">
         <v>10000</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
       </c>
       <c r="E28">
         <v>0.31153846153846099</v>
@@ -1111,9 +1171,15 @@
       <c r="A29" t="s">
         <v>12</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
       <c r="C29">
         <v>100000</v>
       </c>
+      <c r="D29">
+        <v>30</v>
+      </c>
       <c r="E29">
         <v>0.43461538461538402</v>
       </c>
@@ -1123,34 +1189,40 @@
       <c r="G29">
         <v>0.55742448905769504</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31">
-        <v>0.95</v>
-      </c>
-      <c r="C31">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <v>30</v>
-      </c>
-      <c r="E31">
-        <v>0.52108142903121901</v>
-      </c>
-      <c r="F31">
-        <v>0.57578008915304602</v>
-      </c>
-      <c r="G31">
-        <v>0.45737417089348398</v>
-      </c>
-      <c r="H31">
-        <v>-468007.199981982</v>
-      </c>
-      <c r="I31">
-        <v>2.6960000000000002</v>
+      <c r="H29">
+        <v>-102573.40424435301</v>
+      </c>
+      <c r="I29">
+        <v>16.748000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1000000</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>0.52307692307692299</v>
+      </c>
+      <c r="F30">
+        <v>0.55646359583952398</v>
+      </c>
+      <c r="G30">
+        <v>0.46473141616928898</v>
+      </c>
+      <c r="H30">
+        <v>-68005.373123723301</v>
+      </c>
+      <c r="I30">
+        <v>21.210999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1161,25 +1233,25 @@
         <v>0.95</v>
       </c>
       <c r="C32">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>30</v>
       </c>
       <c r="E32">
-        <v>0.52309188138065099</v>
+        <v>0.52108142903121901</v>
       </c>
       <c r="F32">
-        <v>0.57379891035165898</v>
+        <v>0.57578008915304602</v>
       </c>
       <c r="G32">
-        <v>0.45685179743363702</v>
+        <v>0.45737417089348398</v>
       </c>
       <c r="H32">
-        <v>-368356.983215385</v>
+        <v>-468007.199981982</v>
       </c>
       <c r="I32">
-        <v>4.782</v>
+        <v>2.6960000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1190,25 +1262,25 @@
         <v>0.95</v>
       </c>
       <c r="C33">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D33">
         <v>30</v>
       </c>
       <c r="E33">
-        <v>0.55813953488372003</v>
+        <v>0.52309188138065099</v>
       </c>
       <c r="F33">
-        <v>0.622090143635463</v>
+        <v>0.57379891035165898</v>
       </c>
       <c r="G33">
-        <v>0.41661779081133898</v>
+        <v>0.45685179743363702</v>
       </c>
       <c r="H33">
-        <v>-302172.262945308</v>
+        <v>-368356.983215385</v>
       </c>
       <c r="I33">
-        <v>8.4339999999999993</v>
+        <v>4.782</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1219,25 +1291,25 @@
         <v>0.95</v>
       </c>
       <c r="C34">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="D34">
         <v>30</v>
       </c>
       <c r="E34">
-        <v>0.65100893152497497</v>
+        <v>0.55813953488372003</v>
       </c>
       <c r="F34">
-        <v>0.71272907379891004</v>
+        <v>0.622090143635463</v>
       </c>
       <c r="G34">
-        <v>0.32427608092026899</v>
+        <v>0.41661779081133898</v>
       </c>
       <c r="H34">
-        <v>-182849.85858260901</v>
+        <v>-302172.262945308</v>
       </c>
       <c r="I34">
-        <v>15.992000000000001</v>
+        <v>8.4339999999999993</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1248,77 +1320,83 @@
         <v>0.95</v>
       </c>
       <c r="C35">
+        <v>10000</v>
+      </c>
+      <c r="D35">
+        <v>30</v>
+      </c>
+      <c r="E35">
+        <v>0.65100893152497497</v>
+      </c>
+      <c r="F35">
+        <v>0.71272907379891004</v>
+      </c>
+      <c r="G35">
+        <v>0.32427608092026899</v>
+      </c>
+      <c r="H35">
+        <v>-182849.85858260901</v>
+      </c>
+      <c r="I35">
+        <v>15.992000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>0.95</v>
+      </c>
+      <c r="C36">
         <v>100000</v>
       </c>
-      <c r="D35">
-        <v>30</v>
-      </c>
-      <c r="E35">
+      <c r="D36">
+        <v>30</v>
+      </c>
+      <c r="E36">
         <v>0.70938446014127099</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>0.75681030212976697</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>0.27143429487179399</v>
       </c>
-      <c r="H35">
-        <v>-102573.40424435301</v>
-      </c>
-      <c r="I35">
-        <v>16.748000000000001</v>
+      <c r="H36">
+        <v>-103867.225619067</v>
+      </c>
+      <c r="I36">
+        <v>20.273</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37">
-        <v>0.2</v>
+        <v>0.95</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>1000000</v>
+      </c>
+      <c r="D37">
+        <v>30</v>
       </c>
       <c r="E37">
-        <v>0.64011585807385896</v>
+        <v>0.753571428571428</v>
       </c>
       <c r="F37">
-        <v>0.68548786527984096</v>
+        <v>0.77885091629519498</v>
       </c>
       <c r="G37">
-        <v>0.34314173444210899</v>
+        <v>0.23613631780600899</v>
       </c>
       <c r="H37">
-        <v>-467384.686968386</v>
+        <v>-63896.387706943002</v>
       </c>
       <c r="I37">
-        <v>3.2149999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38">
-        <v>0.2</v>
-      </c>
-      <c r="C38">
-        <v>100</v>
-      </c>
-      <c r="E38">
-        <v>0.64288821226620196</v>
-      </c>
-      <c r="F38">
-        <v>0.68623080733036101</v>
-      </c>
-      <c r="G38">
-        <v>0.34110653863740198</v>
-      </c>
-      <c r="H38">
-        <v>-367346.36457428802</v>
-      </c>
-      <c r="I38">
-        <v>5.915</v>
+        <v>25.759</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1329,22 +1407,25 @@
         <v>0.2</v>
       </c>
       <c r="C39">
-        <v>1000</v>
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>30</v>
       </c>
       <c r="E39">
-        <v>0.67101789381050103</v>
+        <v>0.64011585807385896</v>
       </c>
       <c r="F39">
-        <v>0.72065378900445698</v>
+        <v>0.68548786527984096</v>
       </c>
       <c r="G39">
-        <v>0.31051952837140701</v>
+        <v>0.34314173444210899</v>
       </c>
       <c r="H39">
-        <v>-275571.05093552201</v>
+        <v>-467384.686968386</v>
       </c>
       <c r="I39">
-        <v>11.254</v>
+        <v>3.2149999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1355,22 +1436,25 @@
         <v>0.2</v>
       </c>
       <c r="C40">
-        <v>10000</v>
+        <v>100</v>
+      </c>
+      <c r="D40">
+        <v>30</v>
       </c>
       <c r="E40">
-        <v>0.74583517617573303</v>
+        <v>0.64288821226620196</v>
       </c>
       <c r="F40">
-        <v>0.79222387320455601</v>
+        <v>0.68623080733036101</v>
       </c>
       <c r="G40">
-        <v>0.236854264855373</v>
+        <v>0.34110653863740198</v>
       </c>
       <c r="H40">
-        <v>-132033.518239953</v>
+        <v>-367346.36457428802</v>
       </c>
       <c r="I40">
-        <v>19.096</v>
+        <v>5.915</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1381,23 +1465,231 @@
         <v>0.2</v>
       </c>
       <c r="C41">
+        <v>1000</v>
+      </c>
+      <c r="D41">
+        <v>30</v>
+      </c>
+      <c r="E41">
+        <v>0.67101789381050103</v>
+      </c>
+      <c r="F41">
+        <v>0.72065378900445698</v>
+      </c>
+      <c r="G41">
+        <v>0.31051952837140701</v>
+      </c>
+      <c r="H41">
+        <v>-275571.05093552201</v>
+      </c>
+      <c r="I41">
+        <v>11.254</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42">
+        <v>0.2</v>
+      </c>
+      <c r="C42">
+        <v>10000</v>
+      </c>
+      <c r="D42">
+        <v>30</v>
+      </c>
+      <c r="E42">
+        <v>0.74583517617573303</v>
+      </c>
+      <c r="F42">
+        <v>0.79222387320455601</v>
+      </c>
+      <c r="G42">
+        <v>0.236854264855373</v>
+      </c>
+      <c r="H42">
+        <v>-132033.518239953</v>
+      </c>
+      <c r="I42">
+        <v>19.096</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>0.2</v>
+      </c>
+      <c r="C43">
         <v>100000</v>
       </c>
-      <c r="E41">
+      <c r="D43">
+        <v>30</v>
+      </c>
+      <c r="E43">
         <v>0.80552256532066502</v>
       </c>
-      <c r="F41">
+      <c r="F43">
         <v>0.84348687469044004</v>
       </c>
-      <c r="G41">
+      <c r="G43">
         <v>0.18024874698347801</v>
       </c>
-      <c r="H41">
+      <c r="H43">
         <v>-75368.924855253106</v>
       </c>
-      <c r="I41">
+      <c r="I43">
         <v>22.843</v>
       </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>0.2</v>
+      </c>
+      <c r="C44">
+        <v>1000000</v>
+      </c>
+      <c r="D44">
+        <v>30</v>
+      </c>
+      <c r="E44">
+        <v>0.82948278431957001</v>
+      </c>
+      <c r="F44">
+        <v>0.85735512630014798</v>
+      </c>
+      <c r="G44">
+        <v>0.16004466362705799</v>
+      </c>
+      <c r="H44">
+        <v>-54641.825639040799</v>
+      </c>
+      <c r="I44">
+        <v>28.745000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>0.2</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2">
+        <v>30</v>
+      </c>
+      <c r="E46">
+        <v>0.362710990851694</v>
+      </c>
+      <c r="F46">
+        <v>0.44774640911342201</v>
+      </c>
+      <c r="G46">
+        <v>0.60818713450292305</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>0.2</v>
+      </c>
+      <c r="C47">
+        <v>100</v>
+      </c>
+      <c r="D47" s="2">
+        <v>30</v>
+      </c>
+      <c r="E47">
+        <v>0.36966885710604303</v>
+      </c>
+      <c r="F47">
+        <v>0.46260525012382298</v>
+      </c>
+      <c r="G47">
+        <v>0.59852529875413096</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>0.2</v>
+      </c>
+      <c r="C48">
+        <v>1000</v>
+      </c>
+      <c r="D48" s="2">
+        <v>30</v>
+      </c>
+      <c r="E48">
+        <v>0.41760082463600001</v>
+      </c>
+      <c r="F48">
+        <v>0.52674591381872204</v>
+      </c>
+      <c r="G48">
+        <v>0.54504619035511404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49">
+        <v>0.2</v>
+      </c>
+      <c r="C49">
+        <v>10000</v>
+      </c>
+      <c r="D49" s="2">
+        <v>30</v>
+      </c>
+      <c r="E49">
+        <v>0.536915345960572</v>
+      </c>
+      <c r="F49">
+        <v>0.700594353640416</v>
+      </c>
+      <c r="G49">
+        <v>0.40706839562674801</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>0.2</v>
+      </c>
+      <c r="C50">
+        <v>100000</v>
+      </c>
+      <c r="D50" s="2">
+        <v>30</v>
+      </c>
+      <c r="E50">
+        <v>0.60033596071843898</v>
+      </c>
+      <c r="F50">
+        <v>0.76968796433878095</v>
+      </c>
+      <c r="G50">
+        <v>0.34159803005858802</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="D51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>